<commit_message>
proyecto terminado, por ahora
</commit_message>
<xml_diff>
--- a/Presentacion/Resources/Horario-Grupos.xlsx
+++ b/Presentacion/Resources/Horario-Grupos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan-Canseco\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF41F244-F631-4DEB-975C-34802E3F9875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB53BBAC-FF1F-4464-9595-FEA7E4770660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7131F73F-A4CD-4744-A140-CC9546302885}"/>
   </bookViews>
@@ -34,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
-  <si>
-    <t>Secundaria Nuevos Horizontes</t>
-  </si>
-  <si>
-    <t>Horario de clases</t>
-  </si>
-  <si>
-    <t>Ciclo escolar 2024-2025</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Hora</t>
   </si>
@@ -64,9 +55,6 @@
   </si>
   <si>
     <t>7:00 - 8:00</t>
-  </si>
-  <si>
-    <t>Segundo "A"</t>
   </si>
   <si>
     <t>RECESO</t>
@@ -100,7 +88,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +129,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -214,18 +216,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -241,6 +232,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,187 +614,179 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F7051E-F617-48D7-9806-87306AC017E9}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:G14"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="6" width="15.7109375" customWidth="1"/>
+    <col min="2" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="C9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="C12" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="L11" s="9"/>
-    </row>
-    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>